<commit_message>
EPBDS-8724 Simple Rules and Simple Lookups should not support StringRanges for backward compatibility
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-8318_contains.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-8318_contains.xlsx
@@ -646,6 +646,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1108,7 +1109,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="B2:N247"/>
+  <dimension ref="B2:L247"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A204" sqref="A204:XFD247"/>
@@ -1116,14 +1117,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="40.140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="24.28515625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="46.140625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="33.140625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="24.140625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="25.42578125" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="26" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="20.140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" customWidth="true" width="40.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="24.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="46.140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="33.140625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="24.140625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="25.42578125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="26.0" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="20.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
@@ -3471,10 +3472,6 @@
         <v>63</v>
       </c>
       <c r="H164" s="15"/>
-      <c r="K164" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="L164" s="17"/>
     </row>
     <row r="165" spans="2:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B165" s="9" t="s">
@@ -3489,12 +3486,6 @@
       <c r="H165" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="K165" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="L165" s="9" t="s">
-        <v>18</v>
-      </c>
     </row>
     <row r="166" spans="2:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B166" s="2" t="s">
@@ -3507,12 +3498,6 @@
         <v>14</v>
       </c>
       <c r="H166" s="9"/>
-      <c r="K166" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="L166" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="167" spans="2:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B167" s="1" t="s">
@@ -3525,12 +3510,6 @@
         <v>79</v>
       </c>
       <c r="H167" s="9"/>
-      <c r="K167" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="L167" s="1">
-        <v>2</v>
-      </c>
     </row>
     <row r="168" spans="2:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B168" s="1" t="s">
@@ -3545,12 +3524,6 @@
       <c r="H168" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="K168" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="L168" s="1">
-        <v>3</v>
-      </c>
     </row>
     <row r="169" spans="2:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B169" s="1" t="s">
@@ -3565,12 +3538,6 @@
       <c r="H169" s="1">
         <v>1</v>
       </c>
-      <c r="K169" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="L169" s="1">
-        <v>4</v>
-      </c>
     </row>
     <row r="170" spans="2:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B170" s="1" t="s">
@@ -3585,12 +3552,6 @@
       <c r="H170" s="1">
         <v>2</v>
       </c>
-      <c r="K170" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="L170" s="1">
-        <v>5</v>
-      </c>
     </row>
     <row r="171" spans="2:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B171" s="1" t="s">
@@ -3605,12 +3566,6 @@
       <c r="H171" s="1">
         <v>3</v>
       </c>
-      <c r="K171" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="L171" s="1">
-        <v>6</v>
-      </c>
     </row>
     <row r="172" spans="2:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B172" s="1" t="s">
@@ -3625,12 +3580,6 @@
       <c r="H172" s="1">
         <v>4</v>
       </c>
-      <c r="K172" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="L172" s="1">
-        <v>7</v>
-      </c>
     </row>
     <row r="173" spans="2:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B173" s="7" t="s">
@@ -3645,12 +3594,6 @@
       <c r="H173" s="1">
         <v>5</v>
       </c>
-      <c r="K173" s="7" t="s">
-        <v>159</v>
-      </c>
-      <c r="L173" s="7">
-        <v>8</v>
-      </c>
     </row>
     <row r="174" spans="2:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B174" s="7" t="s">
@@ -3665,12 +3608,6 @@
       <c r="H174" s="1">
         <v>6</v>
       </c>
-      <c r="K174" s="7" t="s">
-        <v>160</v>
-      </c>
-      <c r="L174" s="7">
-        <v>9</v>
-      </c>
     </row>
     <row r="175" spans="2:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B175" s="7" t="s">
@@ -3685,12 +3622,6 @@
       <c r="H175" s="1">
         <v>7</v>
       </c>
-      <c r="K175" s="7" t="s">
-        <v>163</v>
-      </c>
-      <c r="L175" s="7">
-        <v>10</v>
-      </c>
     </row>
     <row r="176" spans="2:12" s="6" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B176" s="7" t="s">
@@ -3705,12 +3636,6 @@
       <c r="H176" s="7">
         <v>8</v>
       </c>
-      <c r="K176" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="L176" s="7">
-        <v>11</v>
-      </c>
     </row>
     <row r="177" spans="2:12" s="6" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B177" s="1" t="s">
@@ -3725,12 +3650,6 @@
       <c r="H177" s="7">
         <v>9</v>
       </c>
-      <c r="K177" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="L177" s="7">
-        <v>12</v>
-      </c>
     </row>
     <row r="178" spans="2:12" s="6" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B178" s="1" t="s">
@@ -3744,12 +3663,6 @@
       </c>
       <c r="H178" s="7">
         <v>10</v>
-      </c>
-      <c r="K178" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="L178" s="7">
-        <v>13</v>
       </c>
     </row>
     <row r="179" spans="2:12" s="6" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -3795,10 +3708,6 @@
         <v>186</v>
       </c>
       <c r="H184" s="15"/>
-      <c r="K184" s="15" t="s">
-        <v>187</v>
-      </c>
-      <c r="L184" s="15"/>
     </row>
     <row r="185" spans="2:12" s="6" customFormat="1" ht="14.25" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B185" s="12" t="s">
@@ -3813,12 +3722,6 @@
       <c r="H185" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="K185" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="L185" s="12" t="s">
-        <v>98</v>
-      </c>
     </row>
     <row r="186" spans="2:12" s="6" customFormat="1" ht="14.25" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B186" s="12" t="s">
@@ -3833,12 +3736,6 @@
       <c r="H186" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="K186" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="L186" s="12" t="s">
-        <v>98</v>
-      </c>
     </row>
     <row r="187" spans="2:12" s="6" customFormat="1" ht="14.25" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B187" s="5" t="s">
@@ -3853,12 +3750,6 @@
       <c r="H187" s="5">
         <v>1</v>
       </c>
-      <c r="K187" s="5" t="s">
-        <v>172</v>
-      </c>
-      <c r="L187" s="5">
-        <v>1</v>
-      </c>
     </row>
     <row r="188" spans="2:12" s="6" customFormat="1" ht="14.25" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B188" s="5" t="s">
@@ -3873,12 +3764,6 @@
       <c r="H188" s="5">
         <v>2</v>
       </c>
-      <c r="K188" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="L188" s="5">
-        <v>2</v>
-      </c>
     </row>
     <row r="189" spans="2:12" s="6" customFormat="1" ht="14.25" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B189" s="5" t="s">
@@ -3893,12 +3778,6 @@
       <c r="H189" s="5">
         <v>3</v>
       </c>
-      <c r="K189" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="L189" s="5">
-        <v>3</v>
-      </c>
     </row>
     <row r="190" spans="2:12" s="6" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B190" s="5" t="s">
@@ -3913,12 +3792,6 @@
       <c r="H190" s="5">
         <v>3</v>
       </c>
-      <c r="K190" s="5" t="s">
-        <v>174</v>
-      </c>
-      <c r="L190" s="5">
-        <v>3</v>
-      </c>
     </row>
     <row r="191" spans="2:12" s="6" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B191" s="10" t="s">
@@ -3933,12 +3806,6 @@
       <c r="H191" s="10">
         <v>4</v>
       </c>
-      <c r="K191" s="10" t="s">
-        <v>175</v>
-      </c>
-      <c r="L191" s="10">
-        <v>4</v>
-      </c>
     </row>
     <row r="192" spans="2:12" s="6" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B192" s="10" t="s">
@@ -3953,12 +3820,6 @@
       <c r="H192" s="10">
         <v>5</v>
       </c>
-      <c r="K192" s="10" t="s">
-        <v>176</v>
-      </c>
-      <c r="L192" s="10">
-        <v>5</v>
-      </c>
     </row>
     <row r="193" spans="2:12" s="6" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B193" s="10" t="s">
@@ -3973,12 +3834,6 @@
       <c r="H193" s="10">
         <v>6</v>
       </c>
-      <c r="K193" s="10" t="s">
-        <v>178</v>
-      </c>
-      <c r="L193" s="10">
-        <v>6</v>
-      </c>
     </row>
     <row r="194" spans="2:12" s="6" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B194" s="10" t="s">
@@ -3993,12 +3848,6 @@
       <c r="H194" s="10">
         <v>7</v>
       </c>
-      <c r="K194" s="10" t="s">
-        <v>179</v>
-      </c>
-      <c r="L194" s="10">
-        <v>7</v>
-      </c>
     </row>
     <row r="195" spans="2:12" s="6" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B195" s="10" t="s">
@@ -4013,12 +3862,6 @@
       <c r="H195" s="10">
         <v>8</v>
       </c>
-      <c r="K195" s="10" t="s">
-        <v>180</v>
-      </c>
-      <c r="L195" s="10">
-        <v>8</v>
-      </c>
     </row>
     <row r="196" spans="2:12" s="6" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B196" s="10" t="s">
@@ -4033,12 +3876,6 @@
       <c r="H196" s="10">
         <v>9</v>
       </c>
-      <c r="K196" s="10" t="s">
-        <v>181</v>
-      </c>
-      <c r="L196" s="10">
-        <v>9</v>
-      </c>
     </row>
     <row r="197" spans="2:12" s="6" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B197" s="10" t="s">
@@ -4053,12 +3890,6 @@
       <c r="H197" s="10">
         <v>10</v>
       </c>
-      <c r="K197" s="10" t="s">
-        <v>182</v>
-      </c>
-      <c r="L197" s="10">
-        <v>10</v>
-      </c>
     </row>
     <row r="198" spans="2:12" s="6" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B198" s="10" t="s">
@@ -4073,12 +3904,6 @@
       <c r="H198" s="10">
         <v>11</v>
       </c>
-      <c r="K198" s="10" t="s">
-        <v>183</v>
-      </c>
-      <c r="L198" s="10">
-        <v>11</v>
-      </c>
     </row>
     <row r="199" spans="2:12" s="6" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B199" s="10" t="s">
@@ -4093,12 +3918,6 @@
       <c r="H199" s="10">
         <v>12</v>
       </c>
-      <c r="K199" s="10" t="s">
-        <v>166</v>
-      </c>
-      <c r="L199" s="10">
-        <v>12</v>
-      </c>
     </row>
     <row r="200" spans="2:12" s="6" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B200" s="10" t="s">
@@ -4113,12 +3932,6 @@
       <c r="H200" s="10">
         <v>13</v>
       </c>
-      <c r="K200" s="10" t="s">
-        <v>184</v>
-      </c>
-      <c r="L200" s="10">
-        <v>13</v>
-      </c>
     </row>
     <row r="201" spans="2:12" s="6" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B201" s="10" t="s">
@@ -4131,12 +3944,6 @@
         <v>185</v>
       </c>
       <c r="H201" s="10">
-        <v>13</v>
-      </c>
-      <c r="K201" s="10" t="s">
-        <v>185</v>
-      </c>
-      <c r="L201" s="10">
         <v>13</v>
       </c>
     </row>
@@ -4804,7 +4611,6 @@
     <mergeCell ref="K61:L61"/>
     <mergeCell ref="K39:L39"/>
     <mergeCell ref="G39:H39"/>
-    <mergeCell ref="K164:L164"/>
     <mergeCell ref="B106:C106"/>
     <mergeCell ref="G106:H106"/>
     <mergeCell ref="K106:L106"/>
@@ -4818,7 +4624,6 @@
     <mergeCell ref="K227:L227"/>
     <mergeCell ref="B184:C184"/>
     <mergeCell ref="G184:H184"/>
-    <mergeCell ref="K184:L184"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
EPBDS-9053 Add tests for contains(Range, value) in EPBDS-8318_contains.xlsx file
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-8318_contains.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-8318_contains.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="135" windowWidth="22035" windowHeight="10290"/>
+    <workbookView xWindow="120" yWindow="135" windowWidth="22035" windowHeight="10290" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="235">
   <si>
     <t>Constants</t>
   </si>
@@ -210,9 +210,6 @@
     <t>Rules Integer myRuleString(String a)</t>
   </si>
   <si>
-    <t>SimpleRules  Integer mySimpleRuleString(String a)</t>
-  </si>
-  <si>
     <t>DateRange</t>
   </si>
   <si>
@@ -579,9 +576,6 @@
     <t>Test myRuleString myRuleString_test</t>
   </si>
   <si>
-    <t>Test mySimpleRuleString mySimpleRuleString_test</t>
-  </si>
-  <si>
     <t xml:space="preserve">StringRange test </t>
   </si>
   <si>
@@ -640,13 +634,99 @@
   </si>
   <si>
     <t xml:space="preserve">DateRange test </t>
+  </si>
+  <si>
+    <t>Rules Double myRule_IntRange(Integer a)</t>
+  </si>
+  <si>
+    <t>Rules Double myRule_DoubleRange(Double a)</t>
+  </si>
+  <si>
+    <t>Rules String myRule_StringRange(String a)</t>
+  </si>
+  <si>
+    <t>contains(param, a)</t>
+  </si>
+  <si>
+    <t>IntRange param</t>
+  </si>
+  <si>
+    <t>DoubleRange param</t>
+  </si>
+  <si>
+    <t>StringRange param</t>
+  </si>
+  <si>
+    <t>cond</t>
+  </si>
+  <si>
+    <t>1..2</t>
+  </si>
+  <si>
+    <t>1..1.99</t>
+  </si>
+  <si>
+    <t>2..3</t>
+  </si>
+  <si>
+    <t>3..4</t>
+  </si>
+  <si>
+    <t>Test myRule_IntRange myRule_IntRangeTest</t>
+  </si>
+  <si>
+    <t>Test myRule_DoubleRange myRule_DoubleRangeTest</t>
+  </si>
+  <si>
+    <t>Test myRule_StringRange myRule_StringRangeTest</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>1.98</t>
+  </si>
+  <si>
+    <t>Rules String myRule_CharRange(Character a)</t>
+  </si>
+  <si>
+    <t>Rules String myRule_DateRange(Date a)</t>
+  </si>
+  <si>
+    <t>CharRange param</t>
+  </si>
+  <si>
+    <t>DateRange param</t>
+  </si>
+  <si>
+    <t>01/01/2012..01/01/2013</t>
+  </si>
+  <si>
+    <t>01/01/2013..01/01/2014</t>
+  </si>
+  <si>
+    <t>01/01/2014..01/01/2015</t>
+  </si>
+  <si>
+    <t>Test myRule_CharRange myRule_CharRangeTest</t>
+  </si>
+  <si>
+    <t>Test myRule_DateRange myRule_DateRangeTest</t>
+  </si>
+  <si>
+    <t>Range Contains Test</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -741,7 +821,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
@@ -768,15 +848,22 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1109,30 +1196,30 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="B2:L247"/>
+  <dimension ref="B2:N247"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A204" sqref="A204:XFD247"/>
+    <sheetView topLeftCell="A80" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="40.140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="24.28515625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="46.140625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="33.140625" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="24.140625" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="25.42578125" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="26.0" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="20.140625" collapsed="true"/>
+    <col min="2" max="2" width="40.140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="24.28515625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="46.140625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="33.140625" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="24.140625" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="25.42578125" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="26" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="20.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
@@ -1142,7 +1229,7 @@
         <v>3</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
@@ -1153,7 +1240,7 @@
         <v>4</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="5" spans="2:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -1161,10 +1248,10 @@
         <v>2</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
@@ -1175,7 +1262,7 @@
         <v>9</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
@@ -1301,21 +1388,21 @@
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D19" s="11">
         <v>40238</v>
@@ -1323,21 +1410,21 @@
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>86</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>87</v>
       </c>
       <c r="D21" s="5">
         <v>928371</v>
@@ -1345,13 +1432,13 @@
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>90</v>
-      </c>
       <c r="D22" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
@@ -1359,29 +1446,29 @@
         <v>1</v>
       </c>
       <c r="C23" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D23" s="5" t="s">
         <v>109</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="24" spans="2:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B24" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="25" spans="2:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B25" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="C25" s="7" t="s">
         <v>120</v>
-      </c>
-      <c r="C25" s="7" t="s">
-        <v>121</v>
       </c>
       <c r="D25" s="5">
         <v>21</v>
@@ -1392,10 +1479,10 @@
         <v>7</v>
       </c>
       <c r="C26" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D26" s="5" t="s">
         <v>124</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="27" spans="2:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -1403,10 +1490,10 @@
         <v>38</v>
       </c>
       <c r="C27" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D27" s="5" t="s">
         <v>135</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="28" spans="2:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -1414,10 +1501,10 @@
         <v>53</v>
       </c>
       <c r="C28" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="D28" s="5" t="s">
         <v>161</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="29" spans="2:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -1425,51 +1512,51 @@
         <v>54</v>
       </c>
       <c r="C29" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="D29" s="5" t="s">
         <v>165</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="30" spans="2:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C30" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="D30" s="5" t="s">
         <v>169</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="31" spans="2:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C31" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="D31" s="5" t="s">
         <v>192</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B32" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="33" spans="2:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B33" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D33" s="11">
         <v>41334</v>
@@ -1477,7 +1564,7 @@
     </row>
     <row r="35" spans="2:12" ht="36" collapsed="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B35" s="13" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="36" spans="2:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25"/>
@@ -1492,10 +1579,10 @@
         <v>11</v>
       </c>
       <c r="H39" s="15"/>
-      <c r="K39" s="16" t="s">
+      <c r="K39" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="L39" s="17"/>
+      <c r="L39" s="18"/>
     </row>
     <row r="40" spans="2:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B40" s="9" t="s">
@@ -1537,7 +1624,7 @@
     </row>
     <row r="42" spans="2:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B42" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C42" s="1">
         <v>2</v>
@@ -1547,7 +1634,7 @@
       </c>
       <c r="H42" s="9"/>
       <c r="K42" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="L42" s="1">
         <v>2</v>
@@ -1595,19 +1682,19 @@
     </row>
     <row r="45" spans="2:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B45" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C45" s="1">
         <v>5</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H45" s="1">
         <v>2</v>
       </c>
       <c r="K45" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="L45" s="1">
         <v>5</v>
@@ -1615,7 +1702,7 @@
     </row>
     <row r="46" spans="2:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B46" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C46" s="1">
         <v>6</v>
@@ -1627,7 +1714,7 @@
         <v>3</v>
       </c>
       <c r="K46" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L46" s="1">
         <v>6</v>
@@ -1635,7 +1722,7 @@
     </row>
     <row r="47" spans="2:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B47" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C47" s="7">
         <v>7</v>
@@ -1647,7 +1734,7 @@
         <v>4</v>
       </c>
       <c r="K47" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="L47" s="7">
         <v>7</v>
@@ -1655,19 +1742,19 @@
     </row>
     <row r="48" spans="2:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B48" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C48" s="7">
         <v>8</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H48" s="1">
         <v>5</v>
       </c>
       <c r="K48" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="L48" s="7">
         <v>8</v>
@@ -1675,19 +1762,19 @@
     </row>
     <row r="49" spans="2:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B49" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C49" s="7">
         <v>9</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H49" s="1">
         <v>6</v>
       </c>
       <c r="K49" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L49" s="7">
         <v>9</v>
@@ -1695,19 +1782,19 @@
     </row>
     <row r="50" spans="2:12" s="6" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B50" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C50" s="7">
         <v>10</v>
       </c>
       <c r="G50" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H50" s="7">
         <v>7</v>
       </c>
       <c r="K50" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="L50" s="7">
         <v>10</v>
@@ -1721,7 +1808,7 @@
         <v>11</v>
       </c>
       <c r="G51" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H51" s="7">
         <v>8</v>
@@ -1741,7 +1828,7 @@
         <v>12</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H52" s="7">
         <v>9</v>
@@ -1755,19 +1842,19 @@
     </row>
     <row r="53" spans="2:12" s="6" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B53" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C53" s="7">
         <v>13</v>
       </c>
       <c r="G53" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H53" s="7">
         <v>10</v>
       </c>
       <c r="K53" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="L53" s="7">
         <v>13</v>
@@ -1775,7 +1862,7 @@
     </row>
     <row r="54" spans="2:12" s="6" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B54" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C54" s="7">
         <v>14</v>
@@ -1787,7 +1874,7 @@
         <v>11</v>
       </c>
       <c r="K54" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L54" s="7">
         <v>14</v>
@@ -1803,7 +1890,7 @@
     </row>
     <row r="56" spans="2:12" s="6" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="G56" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H56" s="7">
         <v>13</v>
@@ -1811,7 +1898,7 @@
     </row>
     <row r="57" spans="2:12" s="6" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="G57" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H57" s="7">
         <v>14</v>
@@ -1822,15 +1909,15 @@
     <row r="60" spans="2:12" s="6" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25"/>
     <row r="61" spans="2:12" s="6" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B61" s="15" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C61" s="15"/>
       <c r="G61" s="15" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H61" s="15"/>
       <c r="K61" s="15" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L61" s="15"/>
     </row>
@@ -1839,19 +1926,19 @@
         <v>20</v>
       </c>
       <c r="C62" s="12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G62" s="12" t="s">
         <v>20</v>
       </c>
       <c r="H62" s="12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="K62" s="12" t="s">
         <v>20</v>
       </c>
       <c r="L62" s="12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="63" spans="2:12" s="6" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -1859,19 +1946,19 @@
         <v>20</v>
       </c>
       <c r="C63" s="12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G63" s="12" t="s">
         <v>20</v>
       </c>
       <c r="H63" s="12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="K63" s="12" t="s">
         <v>20</v>
       </c>
       <c r="L63" s="12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="64" spans="2:12" s="6" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -1896,19 +1983,19 @@
     </row>
     <row r="65" spans="2:12" s="6" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B65" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C65" s="5">
         <v>2</v>
       </c>
       <c r="G65" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H65" s="5">
         <v>2</v>
       </c>
       <c r="K65" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="L65" s="5">
         <v>2</v>
@@ -1916,19 +2003,19 @@
     </row>
     <row r="66" spans="2:12" s="6" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B66" s="10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C66" s="5">
         <v>3</v>
       </c>
       <c r="G66" s="10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H66" s="5">
         <v>3</v>
       </c>
       <c r="K66" s="10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L66" s="5">
         <v>3</v>
@@ -1936,19 +2023,19 @@
     </row>
     <row r="67" spans="2:12" s="6" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B67" s="10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C67" s="10">
         <v>4</v>
       </c>
       <c r="G67" s="10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H67" s="10">
         <v>4</v>
       </c>
       <c r="K67" s="10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L67" s="10">
         <v>4</v>
@@ -1956,19 +2043,19 @@
     </row>
     <row r="68" spans="2:12" s="6" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B68" s="10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C68" s="10">
         <v>5</v>
       </c>
       <c r="G68" s="10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H68" s="10">
         <v>5</v>
       </c>
       <c r="K68" s="10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="L68" s="10">
         <v>5</v>
@@ -2016,19 +2103,19 @@
     </row>
     <row r="71" spans="2:12" s="6" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B71" s="10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C71" s="10">
         <v>7</v>
       </c>
       <c r="G71" s="10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H71" s="10">
         <v>7</v>
       </c>
       <c r="K71" s="10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="L71" s="10">
         <v>7</v>
@@ -2056,19 +2143,19 @@
     </row>
     <row r="73" spans="2:12" s="6" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B73" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C73" s="10">
         <v>9</v>
       </c>
       <c r="G73" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H73" s="10">
         <v>9</v>
       </c>
       <c r="K73" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="L73" s="10">
         <v>9</v>
@@ -2076,19 +2163,19 @@
     </row>
     <row r="74" spans="2:12" s="6" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B74" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C74" s="10">
         <v>10</v>
       </c>
       <c r="G74" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H74" s="10">
         <v>10</v>
       </c>
       <c r="K74" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="L74" s="10">
         <v>10</v>
@@ -2096,19 +2183,19 @@
     </row>
     <row r="75" spans="2:12" s="6" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B75" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C75" s="10">
         <v>11</v>
       </c>
       <c r="G75" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H75" s="10">
         <v>11</v>
       </c>
       <c r="K75" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="L75" s="10">
         <v>11</v>
@@ -2116,19 +2203,19 @@
     </row>
     <row r="76" spans="2:12" s="6" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B76" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C76" s="10">
         <v>12</v>
       </c>
       <c r="G76" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H76" s="10">
         <v>12</v>
       </c>
       <c r="K76" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L76" s="10">
         <v>12</v>
@@ -2136,19 +2223,19 @@
     </row>
     <row r="77" spans="2:12" s="6" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B77" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C77" s="10">
         <v>13</v>
       </c>
       <c r="G77" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H77" s="10">
         <v>13</v>
       </c>
       <c r="K77" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="L77" s="10">
         <v>13</v>
@@ -2177,7 +2264,7 @@
     <row r="79" spans="2:12" s="6" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25"/>
     <row r="82" spans="2:12" ht="36" collapsed="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B82" s="13" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="83" spans="2:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25"/>
@@ -2243,7 +2330,7 @@
         <v>2</v>
       </c>
       <c r="G89" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H89" s="9"/>
       <c r="K89" s="1">
@@ -2255,7 +2342,7 @@
     </row>
     <row r="90" spans="2:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B90" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C90" s="1">
         <v>3</v>
@@ -2267,7 +2354,7 @@
         <v>18</v>
       </c>
       <c r="K90" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="L90" s="1">
         <v>3</v>
@@ -2321,7 +2408,7 @@
         <v>6</v>
       </c>
       <c r="G93" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H93" s="1">
         <v>3</v>
@@ -2335,7 +2422,7 @@
     </row>
     <row r="94" spans="2:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B94" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C94" s="7">
         <v>7</v>
@@ -2348,7 +2435,7 @@
         <v>4</v>
       </c>
       <c r="K94" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="L94" s="7">
         <v>7</v>
@@ -2376,7 +2463,7 @@
     </row>
     <row r="96" spans="2:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B96" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C96" s="7">
         <v>9</v>
@@ -2388,7 +2475,7 @@
         <v>6</v>
       </c>
       <c r="K96" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="L96" s="7">
         <v>9</v>
@@ -2396,19 +2483,19 @@
     </row>
     <row r="97" spans="2:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B97" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C97" s="7">
         <v>10</v>
       </c>
       <c r="G97" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H97" s="7">
         <v>7</v>
       </c>
       <c r="K97" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="L97" s="7">
         <v>10</v>
@@ -2416,7 +2503,7 @@
     </row>
     <row r="98" spans="2:12" s="6" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B98" s="7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C98" s="7">
         <v>11</v>
@@ -2428,7 +2515,7 @@
         <v>8</v>
       </c>
       <c r="K98" s="7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="L98" s="7">
         <v>11</v>
@@ -2436,19 +2523,19 @@
     </row>
     <row r="99" spans="2:12" s="6" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B99" s="7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C99" s="7">
         <v>12</v>
       </c>
       <c r="G99" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H99" s="7">
         <v>9</v>
       </c>
       <c r="K99" s="7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="L99" s="7">
         <v>12</v>
@@ -2456,19 +2543,19 @@
     </row>
     <row r="100" spans="2:12" s="6" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B100" s="7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C100" s="7">
         <v>13</v>
       </c>
       <c r="G100" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H100" s="7">
         <v>10</v>
       </c>
       <c r="K100" s="7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="L100" s="7">
         <v>13</v>
@@ -2478,7 +2565,7 @@
       <c r="B101" s="8"/>
       <c r="C101" s="8"/>
       <c r="G101" s="7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H101" s="7">
         <v>11</v>
@@ -2488,7 +2575,7 @@
       <c r="B102" s="8"/>
       <c r="C102" s="8"/>
       <c r="G102" s="7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H102" s="7">
         <v>12</v>
@@ -2498,7 +2585,7 @@
       <c r="B103" s="8"/>
       <c r="C103" s="8"/>
       <c r="G103" s="7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H103" s="7">
         <v>13</v>
@@ -2510,15 +2597,15 @@
     <row r="105" spans="2:12" s="6" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25"/>
     <row r="106" spans="2:12" s="6" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B106" s="15" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C106" s="15"/>
       <c r="G106" s="15" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H106" s="15"/>
       <c r="K106" s="15" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="L106" s="15"/>
     </row>
@@ -2527,19 +2614,19 @@
         <v>20</v>
       </c>
       <c r="C107" s="12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G107" s="12" t="s">
         <v>20</v>
       </c>
       <c r="H107" s="12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="K107" s="12" t="s">
         <v>20</v>
       </c>
       <c r="L107" s="12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="108" spans="2:12" s="6" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -2547,19 +2634,19 @@
         <v>20</v>
       </c>
       <c r="C108" s="12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G108" s="12" t="s">
         <v>20</v>
       </c>
       <c r="H108" s="12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="K108" s="12" t="s">
         <v>20</v>
       </c>
       <c r="L108" s="12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="109" spans="2:12" s="6" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -2806,23 +2893,23 @@
     <row r="122" spans="2:12" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="123" spans="2:12" s="6" customFormat="1" ht="36" collapsed="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B123" s="13" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="124" spans="2:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25"/>
     <row r="125" spans="2:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B125" s="16" t="s">
+      <c r="B125" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="C125" s="17"/>
+      <c r="C125" s="18"/>
       <c r="G125" s="15" t="s">
         <v>48</v>
       </c>
       <c r="H125" s="15"/>
-      <c r="K125" s="16" t="s">
+      <c r="K125" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="L125" s="17"/>
+      <c r="L125" s="18"/>
     </row>
     <row r="126" spans="2:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B126" s="9" t="s">
@@ -2870,7 +2957,7 @@
         <v>2</v>
       </c>
       <c r="G128" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H128" s="1"/>
       <c r="K128" s="1" t="s">
@@ -2963,7 +3050,7 @@
     </row>
     <row r="133" spans="2:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B133" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C133" s="7">
         <v>7</v>
@@ -2975,7 +3062,7 @@
         <v>4</v>
       </c>
       <c r="K133" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L133" s="7">
         <v>7</v>
@@ -3003,7 +3090,7 @@
     </row>
     <row r="135" spans="2:12" s="6" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B135" s="7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C135" s="7">
         <v>9</v>
@@ -3015,7 +3102,7 @@
         <v>6</v>
       </c>
       <c r="K135" s="7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="L135" s="7">
         <v>9</v>
@@ -3023,19 +3110,19 @@
     </row>
     <row r="136" spans="2:12" s="6" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B136" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C136" s="7">
         <v>10</v>
       </c>
       <c r="G136" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H136" s="7">
         <v>7</v>
       </c>
       <c r="K136" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="L136" s="7">
         <v>10</v>
@@ -3043,7 +3130,7 @@
     </row>
     <row r="137" spans="2:12" s="6" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B137" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C137" s="7">
         <v>11</v>
@@ -3055,7 +3142,7 @@
         <v>8</v>
       </c>
       <c r="K137" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L137" s="7">
         <v>11</v>
@@ -3063,19 +3150,19 @@
     </row>
     <row r="138" spans="2:12" s="6" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B138" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C138" s="7">
         <v>12</v>
       </c>
       <c r="G138" s="7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H138" s="7">
         <v>9</v>
       </c>
       <c r="K138" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="L138" s="7">
         <v>12</v>
@@ -3083,19 +3170,19 @@
     </row>
     <row r="139" spans="2:12" s="6" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B139" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C139" s="7">
         <v>13</v>
       </c>
       <c r="G139" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H139" s="7">
         <v>10</v>
       </c>
       <c r="K139" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L139" s="4">
         <v>13</v>
@@ -3105,7 +3192,7 @@
       <c r="B140" s="8"/>
       <c r="C140" s="8"/>
       <c r="G140" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H140" s="7">
         <v>11</v>
@@ -3115,7 +3202,7 @@
       <c r="B141" s="8"/>
       <c r="C141" s="8"/>
       <c r="G141" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H141" s="7">
         <v>12</v>
@@ -3125,7 +3212,7 @@
       <c r="B142" s="8"/>
       <c r="C142" s="8"/>
       <c r="G142" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H142" s="4">
         <v>13</v>
@@ -3141,15 +3228,15 @@
     </row>
     <row r="145" spans="2:12" s="6" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B145" s="15" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C145" s="15"/>
       <c r="G145" s="15" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H145" s="15"/>
       <c r="K145" s="15" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="L145" s="15"/>
     </row>
@@ -3158,19 +3245,19 @@
         <v>20</v>
       </c>
       <c r="C146" s="12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G146" s="12" t="s">
         <v>20</v>
       </c>
       <c r="H146" s="12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="K146" s="12" t="s">
         <v>20</v>
       </c>
       <c r="L146" s="12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="147" spans="2:12" s="6" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -3178,36 +3265,36 @@
         <v>20</v>
       </c>
       <c r="C147" s="12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G147" s="12" t="s">
         <v>20</v>
       </c>
       <c r="H147" s="12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="K147" s="12" t="s">
         <v>20</v>
       </c>
       <c r="L147" s="12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="148" spans="2:12" s="6" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B148" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C148" s="5">
         <v>1</v>
       </c>
       <c r="G148" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H148" s="5">
         <v>1</v>
       </c>
       <c r="K148" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="L148" s="5">
         <v>1</v>
@@ -3235,19 +3322,19 @@
     </row>
     <row r="150" spans="2:12" s="6" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B150" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C150" s="5">
         <v>3</v>
       </c>
       <c r="G150" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H150" s="5">
         <v>3</v>
       </c>
       <c r="K150" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="L150" s="5">
         <v>3</v>
@@ -3255,19 +3342,19 @@
     </row>
     <row r="151" spans="2:12" s="6" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B151" s="5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C151" s="5">
         <v>4</v>
       </c>
       <c r="G151" s="5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H151" s="5">
         <v>4</v>
       </c>
       <c r="K151" s="5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="L151" s="5">
         <v>4</v>
@@ -3295,19 +3382,19 @@
     </row>
     <row r="153" spans="2:12" s="6" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B153" s="10" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C153" s="10">
         <v>6</v>
       </c>
       <c r="G153" s="10" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H153" s="10">
         <v>6</v>
       </c>
       <c r="K153" s="10" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="L153" s="10">
         <v>6</v>
@@ -3315,19 +3402,19 @@
     </row>
     <row r="154" spans="2:12" s="6" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B154" s="10" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C154" s="10">
         <v>7</v>
       </c>
       <c r="G154" s="10" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H154" s="10">
         <v>7</v>
       </c>
       <c r="K154" s="10" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L154" s="10">
         <v>7</v>
@@ -3355,19 +3442,19 @@
     </row>
     <row r="156" spans="2:12" s="6" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B156" s="10" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C156" s="10">
         <v>9</v>
       </c>
       <c r="G156" s="10" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H156" s="10">
         <v>9</v>
       </c>
       <c r="K156" s="10" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="L156" s="10">
         <v>9</v>
@@ -3375,19 +3462,19 @@
     </row>
     <row r="157" spans="2:12" s="6" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B157" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C157" s="10">
         <v>10</v>
       </c>
       <c r="G157" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H157" s="10">
         <v>10</v>
       </c>
       <c r="K157" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="L157" s="10">
         <v>10</v>
@@ -3395,19 +3482,19 @@
     </row>
     <row r="158" spans="2:12" s="6" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B158" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C158" s="10">
         <v>11</v>
       </c>
       <c r="G158" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H158" s="10">
         <v>11</v>
       </c>
       <c r="K158" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="L158" s="10">
         <v>11</v>
@@ -3415,19 +3502,19 @@
     </row>
     <row r="159" spans="2:12" s="6" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B159" s="10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C159" s="10">
         <v>12</v>
       </c>
       <c r="G159" s="10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H159" s="10">
         <v>12</v>
       </c>
       <c r="K159" s="10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="L159" s="10">
         <v>12</v>
@@ -3435,35 +3522,35 @@
     </row>
     <row r="160" spans="2:12" s="6" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B160" s="10" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C160" s="10">
         <v>13</v>
       </c>
       <c r="G160" s="10" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H160" s="10">
         <v>13</v>
       </c>
       <c r="K160" s="10" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="L160" s="10">
         <v>13</v>
       </c>
     </row>
-    <row r="161" spans="2:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="2:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="G161" s="14"/>
       <c r="H161" s="14"/>
     </row>
-    <row r="162" spans="2:12" ht="36" collapsed="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="162" spans="2:8" ht="36" collapsed="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B162" s="13" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="163" spans="2:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25"/>
-    <row r="164" spans="2:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="163" spans="2:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25"/>
+    <row r="164" spans="2:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B164" s="9" t="s">
         <v>62</v>
       </c>
@@ -3473,7 +3560,7 @@
       </c>
       <c r="H164" s="15"/>
     </row>
-    <row r="165" spans="2:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="2:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B165" s="9" t="s">
         <v>20</v>
       </c>
@@ -3487,9 +3574,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="166" spans="2:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="2:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B166" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C166" s="1">
         <v>1</v>
@@ -3499,21 +3586,21 @@
       </c>
       <c r="H166" s="9"/>
     </row>
-    <row r="167" spans="2:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="2:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B167" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C167" s="1">
         <v>2</v>
       </c>
       <c r="G167" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H167" s="9"/>
     </row>
-    <row r="168" spans="2:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="2:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B168" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C168" s="1">
         <v>3</v>
@@ -3525,7 +3612,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="169" spans="2:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="2:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B169" s="1" t="s">
         <v>56</v>
       </c>
@@ -3533,41 +3620,41 @@
         <v>4</v>
       </c>
       <c r="G169" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H169" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="170" spans="2:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="2:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B170" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C170" s="1">
         <v>5</v>
       </c>
       <c r="G170" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H170" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="171" spans="2:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="2:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B171" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C171" s="1">
         <v>6</v>
       </c>
       <c r="G171" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H171" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="172" spans="2:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="2:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B172" s="1" t="s">
         <v>60</v>
       </c>
@@ -3581,37 +3668,37 @@
         <v>4</v>
       </c>
     </row>
-    <row r="173" spans="2:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="2:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B173" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C173" s="7">
         <v>8</v>
       </c>
       <c r="G173" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="H173" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="174" spans="2:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="2:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B174" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C174" s="7">
         <v>9</v>
       </c>
       <c r="G174" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H174" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="175" spans="2:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="2:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B175" s="7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C175" s="7">
         <v>10</v>
@@ -3623,199 +3710,199 @@
         <v>7</v>
       </c>
     </row>
-    <row r="176" spans="2:12" s="6" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="2:8" s="6" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B176" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C176" s="7">
         <v>11</v>
       </c>
       <c r="G176" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H176" s="7">
         <v>8</v>
       </c>
     </row>
-    <row r="177" spans="2:12" s="6" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="2:8" s="6" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B177" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C177" s="7">
         <v>12</v>
       </c>
       <c r="G177" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H177" s="7">
         <v>9</v>
       </c>
     </row>
-    <row r="178" spans="2:12" s="6" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="2:8" s="6" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B178" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C178" s="7">
         <v>13</v>
       </c>
       <c r="G178" s="7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H178" s="7">
         <v>10</v>
       </c>
     </row>
-    <row r="179" spans="2:12" s="6" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="2:8" s="6" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B179" s="14"/>
       <c r="C179" s="8"/>
       <c r="G179" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H179" s="7">
         <v>11</v>
       </c>
     </row>
-    <row r="180" spans="2:12" s="6" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="2:8" s="6" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="G180" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H180" s="7">
         <v>12</v>
       </c>
     </row>
-    <row r="181" spans="2:12" s="6" customFormat="1" ht="14.25" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="2:8" s="6" customFormat="1" ht="14.25" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="G181" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H181" s="7">
         <v>13</v>
       </c>
     </row>
-    <row r="182" spans="2:12" s="6" customFormat="1" ht="14.25" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="2:8" s="6" customFormat="1" ht="14.25" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="G182" s="14"/>
       <c r="H182" s="14"/>
     </row>
-    <row r="183" spans="2:12" s="6" customFormat="1" ht="14.25" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="2:8" s="6" customFormat="1" ht="14.25" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="G183" s="14"/>
       <c r="H183" s="14"/>
     </row>
-    <row r="184" spans="2:12" s="6" customFormat="1" ht="14.25" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="2:8" s="6" customFormat="1" ht="14.25" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B184" s="15" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C184" s="15"/>
       <c r="G184" s="15" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H184" s="15"/>
     </row>
-    <row r="185" spans="2:12" s="6" customFormat="1" ht="14.25" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="2:8" s="6" customFormat="1" ht="14.25" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B185" s="12" t="s">
         <v>20</v>
       </c>
       <c r="C185" s="12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G185" s="12" t="s">
         <v>20</v>
       </c>
       <c r="H185" s="12" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="186" spans="2:12" s="6" customFormat="1" ht="14.25" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="186" spans="2:8" s="6" customFormat="1" ht="14.25" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B186" s="12" t="s">
         <v>20</v>
       </c>
       <c r="C186" s="12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G186" s="12" t="s">
         <v>20</v>
       </c>
       <c r="H186" s="12" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="187" spans="2:12" s="6" customFormat="1" ht="14.25" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="187" spans="2:8" s="6" customFormat="1" ht="14.25" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B187" s="5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C187" s="5">
         <v>1</v>
       </c>
       <c r="G187" s="5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H187" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="188" spans="2:12" s="6" customFormat="1" ht="14.25" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="2:8" s="6" customFormat="1" ht="14.25" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B188" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C188" s="5">
         <v>2</v>
       </c>
       <c r="G188" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H188" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="189" spans="2:12" s="6" customFormat="1" ht="14.25" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="2:8" s="6" customFormat="1" ht="14.25" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B189" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C189" s="5">
         <v>3</v>
       </c>
       <c r="G189" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="H189" s="5">
         <v>3</v>
       </c>
     </row>
-    <row r="190" spans="2:12" s="6" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="2:8" s="6" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B190" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C190" s="5">
         <v>3</v>
       </c>
       <c r="G190" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H190" s="5">
         <v>3</v>
       </c>
     </row>
-    <row r="191" spans="2:12" s="6" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="2:8" s="6" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B191" s="10" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C191" s="10">
         <v>4</v>
       </c>
       <c r="G191" s="10" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H191" s="10">
         <v>4</v>
       </c>
     </row>
-    <row r="192" spans="2:12" s="6" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="2:8" s="6" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B192" s="10" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C192" s="10">
         <v>5</v>
       </c>
       <c r="G192" s="10" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="H192" s="10">
         <v>5</v>
@@ -3823,13 +3910,13 @@
     </row>
     <row r="193" spans="2:12" s="6" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B193" s="10" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C193" s="10">
         <v>6</v>
       </c>
       <c r="G193" s="10" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H193" s="10">
         <v>6</v>
@@ -3837,13 +3924,13 @@
     </row>
     <row r="194" spans="2:12" s="6" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B194" s="10" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C194" s="10">
         <v>7</v>
       </c>
       <c r="G194" s="10" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H194" s="10">
         <v>7</v>
@@ -3851,13 +3938,13 @@
     </row>
     <row r="195" spans="2:12" s="6" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B195" s="10" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C195" s="10">
         <v>8</v>
       </c>
       <c r="G195" s="10" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H195" s="10">
         <v>8</v>
@@ -3865,13 +3952,13 @@
     </row>
     <row r="196" spans="2:12" s="6" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B196" s="10" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C196" s="10">
         <v>9</v>
       </c>
       <c r="G196" s="10" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H196" s="10">
         <v>9</v>
@@ -3879,13 +3966,13 @@
     </row>
     <row r="197" spans="2:12" s="6" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B197" s="10" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C197" s="10">
         <v>10</v>
       </c>
       <c r="G197" s="10" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H197" s="10">
         <v>10</v>
@@ -3893,13 +3980,13 @@
     </row>
     <row r="198" spans="2:12" s="6" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B198" s="10" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C198" s="10">
         <v>11</v>
       </c>
       <c r="G198" s="10" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="H198" s="10">
         <v>11</v>
@@ -3907,13 +3994,13 @@
     </row>
     <row r="199" spans="2:12" s="6" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B199" s="10" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C199" s="10">
         <v>12</v>
       </c>
       <c r="G199" s="10" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H199" s="10">
         <v>12</v>
@@ -3921,13 +4008,13 @@
     </row>
     <row r="200" spans="2:12" s="6" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B200" s="10" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C200" s="10">
         <v>13</v>
       </c>
       <c r="G200" s="10" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="H200" s="10">
         <v>13</v>
@@ -3935,13 +4022,13 @@
     </row>
     <row r="201" spans="2:12" s="6" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B201" s="10" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C201" s="10">
         <v>13</v>
       </c>
       <c r="G201" s="10" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="H201" s="10">
         <v>13</v>
@@ -3954,22 +4041,22 @@
     <row r="203" spans="2:12" collapsed="1" x14ac:dyDescent="0.25"/>
     <row r="204" spans="2:12" s="6" customFormat="1" ht="36" hidden="1" outlineLevel="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B204" s="13" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="205" spans="2:12" s="6" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25"/>
     <row r="206" spans="2:12" s="6" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25"/>
     <row r="207" spans="2:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B207" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C207" s="9"/>
       <c r="G207" s="15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H207" s="15"/>
       <c r="K207" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L207" s="9"/>
     </row>
@@ -3995,17 +4082,17 @@
     </row>
     <row r="209" spans="2:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B209" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C209" s="1">
         <v>1</v>
       </c>
       <c r="G209" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H209" s="9"/>
       <c r="K209" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="L209" s="1">
         <v>1</v>
@@ -4019,7 +4106,7 @@
         <v>2</v>
       </c>
       <c r="G210" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H210" s="9" t="s">
         <v>18</v>
@@ -4033,7 +4120,7 @@
     </row>
     <row r="211" spans="2:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B211" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C211" s="1">
         <v>3</v>
@@ -4045,7 +4132,7 @@
         <v>18</v>
       </c>
       <c r="K211" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="L211" s="1">
         <v>3</v>
@@ -4053,19 +4140,19 @@
     </row>
     <row r="212" spans="2:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B212" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C212" s="1">
         <v>4</v>
       </c>
       <c r="G212" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H212" s="1">
         <v>1</v>
       </c>
       <c r="K212" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="L212" s="1">
         <v>4</v>
@@ -4073,7 +4160,7 @@
     </row>
     <row r="213" spans="2:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B213" s="7" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C213" s="7">
         <v>5</v>
@@ -4085,7 +4172,7 @@
         <v>2</v>
       </c>
       <c r="K213" s="7" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="L213" s="7">
         <v>5</v>
@@ -4093,19 +4180,19 @@
     </row>
     <row r="214" spans="2:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B214" s="7" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C214" s="7">
         <v>6</v>
       </c>
       <c r="G214" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H214" s="1">
         <v>3</v>
       </c>
       <c r="K214" s="7" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="L214" s="7">
         <v>6</v>
@@ -4113,19 +4200,19 @@
     </row>
     <row r="215" spans="2:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B215" s="7" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C215" s="7">
         <v>7</v>
       </c>
       <c r="G215" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H215" s="1">
         <v>4</v>
       </c>
       <c r="K215" s="7" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="L215" s="7">
         <v>7</v>
@@ -4133,19 +4220,19 @@
     </row>
     <row r="216" spans="2:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B216" s="7" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C216" s="7">
         <v>8</v>
       </c>
       <c r="G216" s="7" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="H216" s="7">
         <v>5</v>
       </c>
       <c r="K216" s="7" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="L216" s="7">
         <v>8</v>
@@ -4153,19 +4240,19 @@
     </row>
     <row r="217" spans="2:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B217" s="7" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C217" s="7">
         <v>9</v>
       </c>
       <c r="G217" s="7" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="H217" s="7">
         <v>6</v>
       </c>
       <c r="K217" s="7" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="L217" s="7">
         <v>9</v>
@@ -4173,19 +4260,19 @@
     </row>
     <row r="218" spans="2:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B218" s="7" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C218" s="7">
         <v>10</v>
       </c>
       <c r="G218" s="7" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="H218" s="7">
         <v>7</v>
       </c>
       <c r="K218" s="7" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="L218" s="7">
         <v>10</v>
@@ -4193,19 +4280,19 @@
     </row>
     <row r="219" spans="2:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B219" s="7" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C219" s="7">
         <v>11</v>
       </c>
       <c r="G219" s="7" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="H219" s="7">
         <v>8</v>
       </c>
       <c r="K219" s="7" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="L219" s="7">
         <v>11</v>
@@ -4213,19 +4300,19 @@
     </row>
     <row r="220" spans="2:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B220" s="7" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C220" s="7">
         <v>12</v>
       </c>
       <c r="G220" s="7" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="H220" s="7">
         <v>9</v>
       </c>
       <c r="K220" s="7" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="L220" s="7">
         <v>12</v>
@@ -4233,19 +4320,19 @@
     </row>
     <row r="221" spans="2:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B221" s="1" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C221" s="7">
         <v>13</v>
       </c>
       <c r="G221" s="7" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="H221" s="7">
         <v>10</v>
       </c>
       <c r="K221" s="1" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="L221" s="7">
         <v>13</v>
@@ -4253,7 +4340,7 @@
     </row>
     <row r="222" spans="2:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="G222" s="7" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="H222" s="7">
         <v>11</v>
@@ -4261,7 +4348,7 @@
     </row>
     <row r="223" spans="2:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="G223" s="7" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="H223" s="7">
         <v>12</v>
@@ -4269,7 +4356,7 @@
     </row>
     <row r="224" spans="2:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="G224" s="1" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="H224" s="7">
         <v>13</v>
@@ -4282,15 +4369,15 @@
     <row r="226" spans="2:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25"/>
     <row r="227" spans="2:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B227" s="15" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C227" s="15"/>
       <c r="G227" s="15" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="H227" s="15"/>
       <c r="K227" s="15" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="L227" s="15"/>
     </row>
@@ -4299,19 +4386,19 @@
         <v>20</v>
       </c>
       <c r="C228" s="12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G228" s="12" t="s">
         <v>20</v>
       </c>
       <c r="H228" s="12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="K228" s="12" t="s">
         <v>20</v>
       </c>
       <c r="L228" s="12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="229" spans="2:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -4319,19 +4406,19 @@
         <v>20</v>
       </c>
       <c r="C229" s="12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G229" s="12" t="s">
         <v>20</v>
       </c>
       <c r="H229" s="12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="K229" s="12" t="s">
         <v>20</v>
       </c>
       <c r="L229" s="12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="230" spans="2:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -4516,19 +4603,19 @@
     </row>
     <row r="239" spans="2:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B239" s="5" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C239" s="5">
         <v>10</v>
       </c>
       <c r="G239" s="5" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="H239" s="5">
         <v>10</v>
       </c>
       <c r="K239" s="5" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="L239" s="5">
         <v>10</v>
@@ -4600,30 +4687,30 @@
     <row r="246" spans="2:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25"/>
     <row r="247" spans="2:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="25">
-    <mergeCell ref="G86:H86"/>
-    <mergeCell ref="G125:H125"/>
-    <mergeCell ref="G164:H164"/>
-    <mergeCell ref="G207:H207"/>
-    <mergeCell ref="B61:C61"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="G61:H61"/>
-    <mergeCell ref="K61:L61"/>
-    <mergeCell ref="K39:L39"/>
-    <mergeCell ref="G39:H39"/>
-    <mergeCell ref="B106:C106"/>
-    <mergeCell ref="G106:H106"/>
+  <mergeCells count="23">
+    <mergeCell ref="B227:C227"/>
+    <mergeCell ref="G227:H227"/>
+    <mergeCell ref="K227:L227"/>
+    <mergeCell ref="B184:C184"/>
+    <mergeCell ref="G184:H184"/>
     <mergeCell ref="K106:L106"/>
     <mergeCell ref="B145:C145"/>
     <mergeCell ref="B125:C125"/>
     <mergeCell ref="G145:H145"/>
     <mergeCell ref="K145:L145"/>
     <mergeCell ref="K125:L125"/>
-    <mergeCell ref="B227:C227"/>
-    <mergeCell ref="G227:H227"/>
-    <mergeCell ref="K227:L227"/>
-    <mergeCell ref="B184:C184"/>
-    <mergeCell ref="G184:H184"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="G61:H61"/>
+    <mergeCell ref="K61:L61"/>
+    <mergeCell ref="K39:L39"/>
+    <mergeCell ref="G39:H39"/>
+    <mergeCell ref="G86:H86"/>
+    <mergeCell ref="G125:H125"/>
+    <mergeCell ref="G164:H164"/>
+    <mergeCell ref="G207:H207"/>
+    <mergeCell ref="B61:C61"/>
+    <mergeCell ref="B106:C106"/>
+    <mergeCell ref="G106:H106"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4632,12 +4719,714 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B2:M37"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="2" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="6"/>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B6" s="6"/>
+      <c r="C6" s="19" t="s">
+        <v>206</v>
+      </c>
+      <c r="D6" s="20"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="19" t="s">
+        <v>207</v>
+      </c>
+      <c r="I6" s="20"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="19" t="s">
+        <v>208</v>
+      </c>
+      <c r="M6" s="20"/>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B7" s="6"/>
+      <c r="C7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B8" s="6"/>
+      <c r="C8" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="I8" s="1"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="M8" s="1"/>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B9" s="6"/>
+      <c r="C9" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="D9" s="1"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="I9" s="1"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="M9" s="1"/>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B10" s="6"/>
+      <c r="C10" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B11" s="6"/>
+      <c r="C11" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="D11" s="1">
+        <v>1</v>
+      </c>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="I11" s="1">
+        <v>1</v>
+      </c>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="M11" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B12" s="6"/>
+      <c r="C12" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="D12" s="1">
+        <v>3</v>
+      </c>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="I12" s="1">
+        <v>3</v>
+      </c>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="M12" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B13" s="6"/>
+      <c r="C13" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="D13" s="1">
+        <v>4</v>
+      </c>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="I13" s="1">
+        <v>4</v>
+      </c>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="M13" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="6"/>
+      <c r="M14" s="6"/>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B15" s="6"/>
+      <c r="C15" s="21" t="s">
+        <v>218</v>
+      </c>
+      <c r="D15" s="21"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="21" t="s">
+        <v>219</v>
+      </c>
+      <c r="I15" s="21"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="21" t="s">
+        <v>220</v>
+      </c>
+      <c r="M15" s="21"/>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B16" s="6"/>
+      <c r="C16" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M16" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B17" s="6"/>
+      <c r="C17" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="J17" s="6"/>
+      <c r="K17" s="6"/>
+      <c r="L17" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B18" s="6"/>
+      <c r="C18" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="D18" s="1">
+        <v>1</v>
+      </c>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="I18" s="1">
+        <v>1</v>
+      </c>
+      <c r="J18" s="6"/>
+      <c r="K18" s="6"/>
+      <c r="L18" s="1">
+        <v>1</v>
+      </c>
+      <c r="M18" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B19" s="6"/>
+      <c r="C19" s="1">
+        <v>4</v>
+      </c>
+      <c r="D19" s="1">
+        <v>4</v>
+      </c>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="1">
+        <v>4</v>
+      </c>
+      <c r="I19" s="1">
+        <v>4</v>
+      </c>
+      <c r="J19" s="6"/>
+      <c r="K19" s="6"/>
+      <c r="L19" s="1">
+        <v>4</v>
+      </c>
+      <c r="M19" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="6"/>
+      <c r="K20" s="6"/>
+      <c r="L20" s="6"/>
+      <c r="M20" s="6"/>
+    </row>
+    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6"/>
+      <c r="K21" s="6"/>
+      <c r="L21" s="6"/>
+      <c r="M21" s="6"/>
+    </row>
+    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="6"/>
+      <c r="K22" s="6"/>
+      <c r="L22" s="6"/>
+      <c r="M22" s="6"/>
+    </row>
+    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B23" s="6"/>
+      <c r="C23" s="19" t="s">
+        <v>225</v>
+      </c>
+      <c r="D23" s="20"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="19" t="s">
+        <v>226</v>
+      </c>
+      <c r="I23" s="20"/>
+      <c r="J23" s="6"/>
+      <c r="K23" s="6"/>
+      <c r="L23" s="6"/>
+      <c r="M23" s="6"/>
+    </row>
+    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B24" s="6"/>
+      <c r="C24" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J24" s="6"/>
+      <c r="K24" s="6"/>
+      <c r="L24" s="6"/>
+      <c r="M24" s="6"/>
+    </row>
+    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B25" s="6"/>
+      <c r="C25" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="D25" s="1"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="I25" s="1"/>
+      <c r="J25" s="6"/>
+      <c r="K25" s="6"/>
+      <c r="L25" s="6"/>
+      <c r="M25" s="6"/>
+    </row>
+    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B26" s="6"/>
+      <c r="C26" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="D26" s="1"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="I26" s="1"/>
+      <c r="J26" s="6"/>
+      <c r="K26" s="6"/>
+      <c r="L26" s="6"/>
+      <c r="M26" s="6"/>
+    </row>
+    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B27" s="6"/>
+      <c r="C27" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J27" s="6"/>
+      <c r="K27" s="6"/>
+      <c r="L27" s="6"/>
+      <c r="M27" s="6"/>
+    </row>
+    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B28" s="6"/>
+      <c r="C28" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="D28" s="1">
+        <v>1</v>
+      </c>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="6"/>
+      <c r="H28" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="I28" s="1">
+        <v>1</v>
+      </c>
+      <c r="J28" s="6"/>
+      <c r="K28" s="6"/>
+      <c r="L28" s="6"/>
+      <c r="M28" s="6"/>
+    </row>
+    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B29" s="6"/>
+      <c r="C29" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="D29" s="1">
+        <v>3</v>
+      </c>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="I29" s="1">
+        <v>3</v>
+      </c>
+      <c r="J29" s="6"/>
+      <c r="K29" s="6"/>
+      <c r="L29" s="6"/>
+      <c r="M29" s="6"/>
+    </row>
+    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B30" s="6"/>
+      <c r="C30" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="D30" s="1">
+        <v>4</v>
+      </c>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="6"/>
+      <c r="H30" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="I30" s="1">
+        <v>4</v>
+      </c>
+      <c r="J30" s="6"/>
+      <c r="K30" s="6"/>
+      <c r="L30" s="6"/>
+      <c r="M30" s="6"/>
+    </row>
+    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="6"/>
+      <c r="H31" s="6"/>
+      <c r="I31" s="6"/>
+      <c r="J31" s="6"/>
+      <c r="K31" s="6"/>
+      <c r="L31" s="6"/>
+      <c r="M31" s="6"/>
+    </row>
+    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B32" s="6"/>
+      <c r="C32" s="21" t="s">
+        <v>232</v>
+      </c>
+      <c r="D32" s="21"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="6"/>
+      <c r="G32" s="6"/>
+      <c r="H32" s="21" t="s">
+        <v>233</v>
+      </c>
+      <c r="I32" s="21"/>
+      <c r="J32" s="6"/>
+      <c r="K32" s="6"/>
+      <c r="L32" s="6"/>
+      <c r="M32" s="6"/>
+    </row>
+    <row r="33" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B33" s="6"/>
+      <c r="C33" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="6"/>
+      <c r="H33" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="J33" s="6"/>
+      <c r="K33" s="6"/>
+      <c r="L33" s="6"/>
+      <c r="M33" s="6"/>
+    </row>
+    <row r="34" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B34" s="6"/>
+      <c r="C34" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="E34" s="6"/>
+      <c r="F34" s="6"/>
+      <c r="G34" s="6"/>
+      <c r="H34" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="J34" s="6"/>
+      <c r="K34" s="6"/>
+      <c r="L34" s="6"/>
+      <c r="M34" s="6"/>
+    </row>
+    <row r="35" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B35" s="6"/>
+      <c r="C35" s="1">
+        <v>1</v>
+      </c>
+      <c r="D35" s="1">
+        <v>1</v>
+      </c>
+      <c r="E35" s="6"/>
+      <c r="F35" s="6"/>
+      <c r="G35" s="6"/>
+      <c r="H35" s="3">
+        <v>40918</v>
+      </c>
+      <c r="I35" s="1">
+        <v>1</v>
+      </c>
+      <c r="J35" s="6"/>
+      <c r="K35" s="6"/>
+      <c r="L35" s="6"/>
+      <c r="M35" s="6"/>
+    </row>
+    <row r="36" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B36" s="6"/>
+      <c r="C36" s="1">
+        <v>4</v>
+      </c>
+      <c r="D36" s="1">
+        <v>4</v>
+      </c>
+      <c r="E36" s="6"/>
+      <c r="F36" s="6"/>
+      <c r="G36" s="6"/>
+      <c r="H36" s="3">
+        <v>41649</v>
+      </c>
+      <c r="I36" s="1">
+        <v>4</v>
+      </c>
+      <c r="J36" s="6"/>
+      <c r="K36" s="6"/>
+      <c r="L36" s="6"/>
+      <c r="M36" s="6"/>
+    </row>
+    <row r="37" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B37" s="6"/>
+      <c r="C37" s="6"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="6"/>
+      <c r="F37" s="6"/>
+      <c r="G37" s="6"/>
+      <c r="H37" s="6"/>
+      <c r="I37" s="6"/>
+      <c r="J37" s="6"/>
+      <c r="K37" s="6"/>
+      <c r="L37" s="6"/>
+      <c r="M37" s="6"/>
+    </row>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="H32:I32"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="L6:M6"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="L15:M15"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>